<commit_message>
Query for dps data completed
</commit_message>
<xml_diff>
--- a/files/dps_structured.xlsx
+++ b/files/dps_structured.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Duckie/Documents/Workspace/spcal_2016_github/spcal/private/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Duckie/Documents/Workspace/spcal_2016_github/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,19 +68,19 @@
     <t>AUD</t>
   </si>
   <si>
-    <t>depo_cur</t>
+    <t>conversion_rate</t>
+  </si>
+  <si>
+    <t>interest_rate</t>
+  </si>
+  <si>
+    <t>tenor</t>
   </si>
   <si>
     <t>link_cur</t>
   </si>
   <si>
-    <t>tenor</t>
-  </si>
-  <si>
-    <t>interest_rate</t>
-  </si>
-  <si>
-    <t>conversion_rate</t>
+    <t>depo_cur</t>
   </si>
 </sst>
 </file>
@@ -127,14 +127,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,33 +416,26 @@
   <dimension ref="A1:E513"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:E513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>16</v>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -455,7 +449,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E2">
         <v>5.9015000000000004</v>
@@ -472,7 +466,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>5.9054000000000002</v>
@@ -489,7 +483,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E4">
         <v>5.9089999999999998</v>
@@ -506,7 +500,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>5.9123999999999999</v>
@@ -523,7 +517,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E6">
         <v>5.9157000000000002</v>
@@ -540,7 +534,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E7">
         <v>5.9188000000000001</v>
@@ -557,7 +551,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E8">
         <v>5.9218000000000002</v>
@@ -574,7 +568,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E9">
         <v>5.9245999999999999</v>
@@ -591,7 +585,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E10">
         <v>5.9273999999999996</v>
@@ -608,7 +602,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E11">
         <v>5.8937999999999997</v>
@@ -625,7 +619,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E12">
         <v>5.9006999999999996</v>
@@ -642,7 +636,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E13">
         <v>5.9071999999999996</v>
@@ -659,7 +653,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <v>5.9131999999999998</v>
@@ -676,7 +670,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E15">
         <v>5.9189999999999996</v>
@@ -693,7 +687,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E16">
         <v>5.9244000000000003</v>
@@ -710,7 +704,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E17">
         <v>5.9295999999999998</v>
@@ -727,7 +721,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E18">
         <v>5.9344999999999999</v>
@@ -744,7 +738,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E19">
         <v>5.9391999999999996</v>
@@ -761,7 +755,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E20">
         <v>5.8960999999999997</v>
@@ -778,7 +772,7 @@
         <v>5</v>
       </c>
       <c r="D21" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E21">
         <v>5.9055</v>
@@ -795,7 +789,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E22">
         <v>5.9142000000000001</v>
@@ -812,7 +806,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E23">
         <v>5.9222999999999999</v>
@@ -829,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E24">
         <v>5.93</v>
@@ -846,7 +840,7 @@
         <v>5</v>
       </c>
       <c r="D25" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E25">
         <v>5.9371999999999998</v>
@@ -863,7 +857,7 @@
         <v>5</v>
       </c>
       <c r="D26" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E26">
         <v>5.9440999999999997</v>
@@ -880,7 +874,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E27">
         <v>5.9507000000000003</v>
@@ -897,7 +891,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E28">
         <v>5.9569999999999999</v>
@@ -914,7 +908,7 @@
         <v>4</v>
       </c>
       <c r="D29" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E29">
         <v>5.8940000000000001</v>
@@ -931,7 +925,7 @@
         <v>4</v>
       </c>
       <c r="D30" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E30">
         <v>5.9059999999999997</v>
@@ -948,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="D31" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E31">
         <v>5.9170999999999996</v>
@@ -965,7 +959,7 @@
         <v>4</v>
       </c>
       <c r="D32" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E32">
         <v>5.9273999999999996</v>
@@ -982,7 +976,7 @@
         <v>4</v>
       </c>
       <c r="D33" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E33">
         <v>5.9371</v>
@@ -999,7 +993,7 @@
         <v>4</v>
       </c>
       <c r="D34" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E34">
         <v>5.9462000000000002</v>
@@ -1016,7 +1010,7 @@
         <v>4</v>
       </c>
       <c r="D35" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E35">
         <v>5.9549000000000003</v>
@@ -1033,7 +1027,7 @@
         <v>4</v>
       </c>
       <c r="D36" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E36">
         <v>5.9631999999999996</v>
@@ -1050,7 +1044,7 @@
         <v>3</v>
       </c>
       <c r="D37" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E37" s="3">
         <v>5.915</v>
@@ -1067,7 +1061,7 @@
         <v>3</v>
       </c>
       <c r="D38" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E38" s="3">
         <v>5.9362000000000004</v>
@@ -1084,7 +1078,7 @@
         <v>3</v>
       </c>
       <c r="D39" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E39" s="3">
         <v>5.9558999999999997</v>
@@ -1101,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="D40" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E40" s="3">
         <v>5.9401000000000002</v>
@@ -1118,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="D41" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E41" s="3">
         <v>5.9683000000000002</v>
@@ -1135,7 +1129,7 @@
         <v>7</v>
       </c>
       <c r="D42" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E42" s="1">
         <v>0.16944844531051426</v>
@@ -1152,7 +1146,7 @@
         <v>7</v>
       </c>
       <c r="D43" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E43" s="1">
         <v>0.16933653943848004</v>
@@ -1169,7 +1163,7 @@
         <v>7</v>
       </c>
       <c r="D44" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E44" s="1">
         <v>0.16923337282112033</v>
@@ -1186,7 +1180,7 @@
         <v>7</v>
       </c>
       <c r="D45" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E45" s="1">
         <v>0.16913605304106624</v>
@@ -1203,7 +1197,7 @@
         <v>7</v>
       </c>
       <c r="D46" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E46" s="1">
         <v>0.16904170258802848</v>
@@ -1220,7 +1214,7 @@
         <v>7</v>
       </c>
       <c r="D47" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E47" s="1">
         <v>0.16895316618233425</v>
@@ -1237,7 +1231,7 @@
         <v>7</v>
       </c>
       <c r="D48" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E48" s="1">
         <v>0.16886757404843122</v>
@@ -1254,7 +1248,7 @@
         <v>7</v>
       </c>
       <c r="D49" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E49" s="1">
         <v>0.16878776626270128</v>
@@ -1271,7 +1265,7 @@
         <v>7</v>
       </c>
       <c r="D50" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E50" s="1">
         <v>0.16870803387657321</v>
@@ -1288,7 +1282,7 @@
         <v>6</v>
       </c>
       <c r="D51" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E51" s="1">
         <v>0.16966982252536564</v>
@@ -1305,7 +1299,7 @@
         <v>6</v>
       </c>
       <c r="D52" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E52" s="1">
         <v>0.16947141864524548</v>
@@ -1322,7 +1316,7 @@
         <v>6</v>
       </c>
       <c r="D53" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E53" s="1">
         <v>0.169284940411701</v>
@@ -1339,7 +1333,7 @@
         <v>6</v>
       </c>
       <c r="D54" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E54" s="1">
         <v>0.16911317053372119</v>
@@ -1356,7 +1350,7 @@
         <v>6</v>
       </c>
       <c r="D55" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E55" s="1">
         <v>0.16894745734076702</v>
@@ -1373,7 +1367,7 @@
         <v>6</v>
       </c>
       <c r="D56" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E56" s="1">
         <v>0.16879346431706163</v>
@@ -1390,7 +1384,7 @@
         <v>6</v>
       </c>
       <c r="D57" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E57" s="1">
         <v>0.16864543982730706</v>
@@ -1407,7 +1401,7 @@
         <v>6</v>
       </c>
       <c r="D58" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E58" s="1">
         <v>0.16850619260257815</v>
@@ -1424,7 +1418,7 @@
         <v>6</v>
       </c>
       <c r="D59" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E59" s="1">
         <v>0.16837284482758622</v>
@@ -1441,7 +1435,7 @@
         <v>5</v>
       </c>
       <c r="D60" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E60" s="1">
         <v>0.16960363630196232</v>
@@ -1458,7 +1452,7 @@
         <v>5</v>
       </c>
       <c r="D61" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E61" s="1">
         <v>0.16933367200067734</v>
@@ -1475,7 +1469,7 @@
         <v>5</v>
       </c>
       <c r="D62" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E62" s="1">
         <v>0.16908457610496769</v>
@@ -1492,7 +1486,7 @@
         <v>5</v>
       </c>
       <c r="D63" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E63" s="1">
         <v>0.16885331712341489</v>
@@ -1509,7 +1503,7 @@
         <v>5</v>
       </c>
       <c r="D64" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E64" s="1">
         <v>0.16863406408094436</v>
@@ -1526,7 +1520,7 @@
         <v>5</v>
       </c>
       <c r="D65" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E65" s="1">
         <v>0.16842956275685508</v>
@@ -1543,7 +1537,7 @@
         <v>5</v>
       </c>
       <c r="D66" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E66" s="1">
         <v>0.16823404720647364</v>
@@ -1560,7 +1554,7 @@
         <v>5</v>
       </c>
       <c r="D67" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E67" s="1">
         <v>0.16804745660174433</v>
@@ -1577,7 +1571,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E68" s="1">
         <v>0.16786973308712438</v>
@@ -1594,7 +1588,7 @@
         <v>4</v>
       </c>
       <c r="D69" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E69" s="1">
         <v>0.16966406515100102</v>
@@ -1611,7 +1605,7 @@
         <v>4</v>
       </c>
       <c r="D70" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E70" s="1">
         <v>0.16931933626820184</v>
@@ -1628,7 +1622,7 @@
         <v>4</v>
       </c>
       <c r="D71" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E71" s="1">
         <v>0.16900170691723987</v>
@@ -1645,7 +1639,7 @@
         <v>4</v>
       </c>
       <c r="D72" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E72" s="1">
         <v>0.16870803387657321</v>
@@ -1662,7 +1656,7 @@
         <v>4</v>
       </c>
       <c r="D73" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E73" s="1">
         <v>0.16843239965639789</v>
@@ -1679,7 +1673,7 @@
         <v>4</v>
       </c>
       <c r="D74" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E74" s="1">
         <v>0.1681746325384279</v>
@@ -1696,7 +1690,7 @@
         <v>4</v>
       </c>
       <c r="D75" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E75" s="1">
         <v>0.16792893247577625</v>
@@ -1713,7 +1707,7 @@
         <v>4</v>
       </c>
       <c r="D76" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E76" s="1">
         <v>0.16769519720955192</v>
@@ -1730,7 +1724,7 @@
         <v>3</v>
       </c>
       <c r="D77" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E77" s="1">
         <v>0.16906170752324598</v>
@@ -1747,7 +1741,7 @@
         <v>3</v>
       </c>
       <c r="D78" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E78" s="1">
         <v>0.16845793605336745</v>
@@ -1764,7 +1758,7 @@
         <v>3</v>
       </c>
       <c r="D79" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E79" s="1">
         <v>0.16790073708423581</v>
@@ -1781,7 +1775,7 @@
         <v>0</v>
       </c>
       <c r="D80" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E80" s="1">
         <v>0.16834733421996262</v>
@@ -1798,7 +1792,7 @@
         <v>0</v>
       </c>
       <c r="D81" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E81" s="1">
         <v>0.16755189920077743</v>
@@ -1815,7 +1809,7 @@
         <v>7</v>
       </c>
       <c r="D82" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E82" s="1">
         <v>0.75939999999999996</v>
@@ -1832,7 +1826,7 @@
         <v>7</v>
       </c>
       <c r="D83" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E83" s="1">
         <v>0.76</v>
@@ -1849,7 +1843,7 @@
         <v>7</v>
       </c>
       <c r="D84" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E84" s="1">
         <v>0.76060000000000005</v>
@@ -1866,7 +1860,7 @@
         <v>7</v>
       </c>
       <c r="D85" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E85" s="1">
         <v>0.7611</v>
@@ -1883,7 +1877,7 @@
         <v>7</v>
       </c>
       <c r="D86" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E86" s="1">
         <v>0.76160000000000005</v>
@@ -1900,7 +1894,7 @@
         <v>7</v>
       </c>
       <c r="D87" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E87" s="1">
         <v>0.7621</v>
@@ -1917,7 +1911,7 @@
         <v>7</v>
       </c>
       <c r="D88" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E88" s="1">
         <v>0.76249999999999996</v>
@@ -1934,7 +1928,7 @@
         <v>7</v>
       </c>
       <c r="D89" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E89" s="1">
         <v>0.76290000000000002</v>
@@ -1951,7 +1945,7 @@
         <v>7</v>
       </c>
       <c r="D90" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E90" s="1">
         <v>0.76329999999999998</v>
@@ -1968,7 +1962,7 @@
         <v>6</v>
       </c>
       <c r="D91" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E91" s="1">
         <v>0.75890000000000002</v>
@@ -1985,7 +1979,7 @@
         <v>6</v>
       </c>
       <c r="D92" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E92" s="1">
         <v>0.75990000000000002</v>
@@ -2002,7 +1996,7 @@
         <v>6</v>
       </c>
       <c r="D93" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E93" s="1">
         <v>0.76080000000000003</v>
@@ -2019,7 +2013,7 @@
         <v>6</v>
       </c>
       <c r="D94" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E94" s="1">
         <v>0.76170000000000004</v>
@@ -2036,7 +2030,7 @@
         <v>6</v>
       </c>
       <c r="D95" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E95" s="1">
         <v>0.76249999999999996</v>
@@ -2053,7 +2047,7 @@
         <v>6</v>
       </c>
       <c r="D96" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E96" s="1">
         <v>0.76319999999999999</v>
@@ -2070,7 +2064,7 @@
         <v>6</v>
       </c>
       <c r="D97" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E97" s="1">
         <v>0.76390000000000002</v>
@@ -2087,7 +2081,7 @@
         <v>6</v>
       </c>
       <c r="D98" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E98" s="1">
         <v>0.76459999999999995</v>
@@ -2104,7 +2098,7 @@
         <v>6</v>
       </c>
       <c r="D99" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E99" s="1">
         <v>0.76529999999999998</v>
@@ -2121,7 +2115,7 @@
         <v>5</v>
       </c>
       <c r="D100" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E100" s="1">
         <v>0.75829999999999997</v>
@@ -2138,7 +2132,7 @@
         <v>5</v>
       </c>
       <c r="D101" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E101" s="1">
         <v>0.75970000000000004</v>
@@ -2155,7 +2149,7 @@
         <v>5</v>
       </c>
       <c r="D102" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E102" s="1">
         <v>0.76090000000000002</v>
@@ -2172,7 +2166,7 @@
         <v>5</v>
       </c>
       <c r="D103" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E103" s="1">
         <v>0.7621</v>
@@ -2189,7 +2183,7 @@
         <v>5</v>
       </c>
       <c r="D104" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E104" s="1">
         <v>0.76319999999999999</v>
@@ -2206,7 +2200,7 @@
         <v>5</v>
       </c>
       <c r="D105" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E105" s="1">
         <v>0.76429999999999998</v>
@@ -2223,7 +2217,7 @@
         <v>5</v>
       </c>
       <c r="D106" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E106" s="1">
         <v>0.76519999999999999</v>
@@ -2240,7 +2234,7 @@
         <v>5</v>
       </c>
       <c r="D107" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E107" s="1">
         <v>0.76619999999999999</v>
@@ -2257,7 +2251,7 @@
         <v>5</v>
       </c>
       <c r="D108" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E108" s="1">
         <v>0.76700000000000002</v>
@@ -2274,7 +2268,7 @@
         <v>4</v>
       </c>
       <c r="D109" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E109" s="1">
         <v>0.75770000000000004</v>
@@ -2291,7 +2285,7 @@
         <v>4</v>
       </c>
       <c r="D110" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E110" s="1">
         <v>0.75949999999999995</v>
@@ -2308,7 +2302,7 @@
         <v>4</v>
       </c>
       <c r="D111" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E111" s="1">
         <v>0.7611</v>
@@ -2325,7 +2319,7 @@
         <v>4</v>
       </c>
       <c r="D112" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E112" s="1">
         <v>0.76259999999999994</v>
@@ -2342,7 +2336,7 @@
         <v>4</v>
       </c>
       <c r="D113" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E113" s="1">
         <v>0.76400000000000001</v>
@@ -2359,7 +2353,7 @@
         <v>4</v>
       </c>
       <c r="D114" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E114" s="1">
         <v>0.76529999999999998</v>
@@ -2376,7 +2370,7 @@
         <v>4</v>
       </c>
       <c r="D115" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E115" s="1">
         <v>0.76649999999999996</v>
@@ -2393,7 +2387,7 @@
         <v>4</v>
       </c>
       <c r="D116" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E116" s="1">
         <v>0.76759999999999995</v>
@@ -2410,7 +2404,7 @@
         <v>4</v>
       </c>
       <c r="D117" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E117" s="1">
         <v>0.76870000000000005</v>
@@ -2427,7 +2421,7 @@
         <v>3</v>
       </c>
       <c r="D118" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E118" s="1">
         <v>0.75960000000000005</v>
@@ -2444,7 +2438,7 @@
         <v>3</v>
       </c>
       <c r="D119" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E119" s="1">
         <v>0.76270000000000004</v>
@@ -2461,7 +2455,7 @@
         <v>3</v>
       </c>
       <c r="D120" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E120" s="1">
         <v>0.76549999999999996</v>
@@ -2478,7 +2472,7 @@
         <v>3</v>
       </c>
       <c r="D121" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E121" s="1">
         <v>0.7681</v>
@@ -2495,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="D122" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E122" s="1">
         <v>0.76160000000000005</v>
@@ -2512,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="D123" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E123" s="1">
         <v>0.76580000000000004</v>
@@ -2529,7 +2523,7 @@
         <v>0</v>
       </c>
       <c r="D124" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E124" s="1">
         <v>0.76959999999999995</v>
@@ -2546,7 +2540,7 @@
         <v>7</v>
       </c>
       <c r="D125" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E125" s="1">
         <v>1.3168290755859891</v>
@@ -2563,7 +2557,7 @@
         <v>7</v>
       </c>
       <c r="D126" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E126" s="1">
         <v>1.3157894736842106</v>
@@ -2580,7 +2574,7 @@
         <v>7</v>
       </c>
       <c r="D127" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E127" s="1">
         <v>1.3147515119642386</v>
@@ -2597,7 +2591,7 @@
         <v>7</v>
       </c>
       <c r="D128" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E128" s="1">
         <v>1.3138877939823939</v>
@@ -2614,7 +2608,7 @@
         <v>7</v>
       </c>
       <c r="D129" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E129" s="1">
         <v>1.3130252100840336</v>
@@ -2631,7 +2625,7 @@
         <v>7</v>
       </c>
       <c r="D130" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E130" s="1">
         <v>1.3121637580370029</v>
@@ -2648,7 +2642,7 @@
         <v>7</v>
       </c>
       <c r="D131" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E131" s="1">
         <v>1.3114754098360657</v>
@@ -2665,7 +2659,7 @@
         <v>7</v>
       </c>
       <c r="D132" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E132" s="1">
         <v>1.3107877834578581</v>
@@ -2682,7 +2676,7 @@
         <v>7</v>
       </c>
       <c r="D133" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E133" s="1">
         <v>1.3101008777675882</v>
@@ -2699,7 +2693,7 @@
         <v>6</v>
       </c>
       <c r="D134" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E134" s="1">
         <v>1.3176966662274343</v>
@@ -2716,7 +2710,7 @@
         <v>6</v>
       </c>
       <c r="D135" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E135" s="1">
         <v>1.3159626266614028</v>
@@ -2733,7 +2727,7 @@
         <v>6</v>
       </c>
       <c r="D136" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E136" s="1">
         <v>1.3144058885383807</v>
@@ -2750,7 +2744,7 @@
         <v>6</v>
       </c>
       <c r="D137" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E137" s="1">
         <v>1.3128528291978467</v>
@@ -2767,7 +2761,7 @@
         <v>6</v>
       </c>
       <c r="D138" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E138" s="1">
         <v>1.3114754098360657</v>
@@ -2784,7 +2778,7 @@
         <v>6</v>
       </c>
       <c r="D139" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E139" s="1">
         <v>1.3102725366876311</v>
@@ -2801,7 +2795,7 @@
         <v>6</v>
       </c>
       <c r="D140" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E140" s="1">
         <v>1.3090718680455558</v>
@@ -2818,7 +2812,7 @@
         <v>6</v>
       </c>
       <c r="D141" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E141" s="1">
         <v>1.3078733978550878</v>
@@ -2835,7 +2829,7 @@
         <v>6</v>
       </c>
       <c r="D142" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E142" s="1">
         <v>1.3066771200836274</v>
@@ -2852,7 +2846,7 @@
         <v>5</v>
       </c>
       <c r="D143" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E143" s="1">
         <v>1.3187392852433075</v>
@@ -2869,7 +2863,7 @@
         <v>5</v>
       </c>
       <c r="D144" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E144" s="1">
         <v>1.3163090693694879</v>
@@ -2886,7 +2880,7 @@
         <v>5</v>
       </c>
       <c r="D145" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E145" s="1">
         <v>1.3142331449599158</v>
@@ -2903,7 +2897,7 @@
         <v>5</v>
       </c>
       <c r="D146" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E146" s="1">
         <v>1.3121637580370029</v>
@@ -2920,7 +2914,7 @@
         <v>5</v>
       </c>
       <c r="D147" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E147" s="1">
         <v>1.3102725366876311</v>
@@ -2937,7 +2931,7 @@
         <v>5</v>
       </c>
       <c r="D148" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E148" s="1">
         <v>1.3083867591259977</v>
@@ -2954,7 +2948,7 @@
         <v>5</v>
       </c>
       <c r="D149" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E149" s="1">
         <v>1.3068478829064296</v>
@@ -2971,7 +2965,7 @@
         <v>5</v>
       </c>
       <c r="D150" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E150" s="1">
         <v>1.3051422605063951</v>
@@ -2988,7 +2982,7 @@
         <v>5</v>
       </c>
       <c r="D151" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E151" s="1">
         <v>1.3037809647979139</v>
@@ -3005,7 +2999,7 @@
         <v>4</v>
       </c>
       <c r="D152" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E152" s="1">
         <v>1.3197835554968984</v>
@@ -3022,7 +3016,7 @@
         <v>4</v>
       </c>
       <c r="D153" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E153" s="1">
         <v>1.3166556945358789</v>
@@ -3039,7 +3033,7 @@
         <v>4</v>
       </c>
       <c r="D154" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E154" s="1">
         <v>1.3138877939823939</v>
@@ -3056,7 +3050,7 @@
         <v>4</v>
       </c>
       <c r="D155" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E155" s="1">
         <v>1.3113034356150015</v>
@@ -3073,7 +3067,7 @@
         <v>4</v>
       </c>
       <c r="D156" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E156" s="1">
         <v>1.3089005235602094</v>
@@ -3090,7 +3084,7 @@
         <v>4</v>
       </c>
       <c r="D157" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E157" s="1">
         <v>1.3066771200836274</v>
@@ -3107,7 +3101,7 @@
         <v>4</v>
       </c>
       <c r="D158" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E158" s="1">
         <v>1.3046314416177431</v>
@@ -3124,7 +3118,7 @@
         <v>4</v>
       </c>
       <c r="D159" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E159" s="1">
         <v>1.3027618551328819</v>
@@ -3141,7 +3135,7 @@
         <v>4</v>
       </c>
       <c r="D160" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E160" s="1">
         <v>1.3008976193573565</v>
@@ -3158,7 +3152,7 @@
         <v>3</v>
       </c>
       <c r="D161" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E161" s="1">
         <v>1.3164823591363874</v>
@@ -3175,7 +3169,7 @@
         <v>3</v>
       </c>
       <c r="D162" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E162" s="1">
         <v>1.3111315064901008</v>
@@ -3192,7 +3186,7 @@
         <v>3</v>
       </c>
       <c r="D163" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E163" s="1">
         <v>1.3063357282821686</v>
@@ -3209,7 +3203,7 @@
         <v>3</v>
       </c>
       <c r="D164" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E164" s="1">
         <v>1.3019138133055592</v>
@@ -3226,7 +3220,7 @@
         <v>0</v>
       </c>
       <c r="D165" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E165" s="1">
         <v>1.3130252100840336</v>
@@ -3243,7 +3237,7 @@
         <v>0</v>
       </c>
       <c r="D166" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E166" s="1">
         <v>1.3058239749281797</v>
@@ -3260,7 +3254,7 @@
         <v>0</v>
       </c>
       <c r="D167" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E167" s="1">
         <v>1.2993762993762994</v>
@@ -3277,7 +3271,7 @@
         <v>7</v>
       </c>
       <c r="D168" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E168" s="1">
         <v>9.7532999999999994</v>
@@ -3294,7 +3288,7 @@
         <v>7</v>
       </c>
       <c r="D169" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E169" s="1">
         <v>9.7475000000000005</v>
@@ -3311,7 +3305,7 @@
         <v>7</v>
       </c>
       <c r="D170" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E170" s="1">
         <v>9.7418999999999993</v>
@@ -3328,7 +3322,7 @@
         <v>7</v>
       </c>
       <c r="D171" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E171" s="1">
         <v>9.7367000000000008</v>
@@ -3345,7 +3339,7 @@
         <v>7</v>
       </c>
       <c r="D172" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E172" s="1">
         <v>9.7317</v>
@@ -3362,7 +3356,7 @@
         <v>7</v>
       </c>
       <c r="D173" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E173" s="1">
         <v>9.7268000000000008</v>
@@ -3379,7 +3373,7 @@
         <v>7</v>
       </c>
       <c r="D174" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E174" s="1">
         <v>9.7222000000000008</v>
@@ -3396,7 +3390,7 @@
         <v>7</v>
       </c>
       <c r="D175" s="2">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="E175" s="1">
         <v>9.7177000000000007</v>
@@ -3413,7 +3407,7 @@
         <v>7</v>
       </c>
       <c r="D176" s="2">
-        <v>9.5000000000000001E-2</v>
+        <v>9.5</v>
       </c>
       <c r="E176" s="1">
         <v>9.7134</v>
@@ -3430,7 +3424,7 @@
         <v>6</v>
       </c>
       <c r="D177" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E177" s="1">
         <v>9.7583000000000002</v>
@@ -3447,7 +3441,7 @@
         <v>6</v>
       </c>
       <c r="D178" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E178" s="1">
         <v>9.7482000000000006</v>
@@ -3464,7 +3458,7 @@
         <v>6</v>
       </c>
       <c r="D179" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E179" s="1">
         <v>9.7386999999999997</v>
@@ -3481,7 +3475,7 @@
         <v>6</v>
       </c>
       <c r="D180" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E180" s="1">
         <v>9.7297999999999991</v>
@@ -3498,7 +3492,7 @@
         <v>6</v>
       </c>
       <c r="D181" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E181" s="1">
         <v>9.7211999999999996</v>
@@ -3515,7 +3509,7 @@
         <v>6</v>
       </c>
       <c r="D182" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E182" s="1">
         <v>9.7129999999999992</v>
@@ -3532,7 +3526,7 @@
         <v>6</v>
       </c>
       <c r="D183" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E183" s="1">
         <v>9.7051999999999996</v>
@@ -3549,7 +3543,7 @@
         <v>6</v>
       </c>
       <c r="D184" s="2">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="E184" s="1">
         <v>9.6975999999999996</v>
@@ -3566,7 +3560,7 @@
         <v>6</v>
       </c>
       <c r="D185" s="2">
-        <v>9.5000000000000001E-2</v>
+        <v>9.5</v>
       </c>
       <c r="E185" s="1">
         <v>9.6903000000000006</v>
@@ -3583,7 +3577,7 @@
         <v>5</v>
       </c>
       <c r="D186" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E186" s="1">
         <v>9.7561</v>
@@ -3600,7 +3594,7 @@
         <v>5</v>
       </c>
       <c r="D187" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E187" s="1">
         <v>9.7423999999999999</v>
@@ -3617,7 +3611,7 @@
         <v>5</v>
       </c>
       <c r="D188" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E188" s="1">
         <v>9.7295999999999996</v>
@@ -3634,7 +3628,7 @@
         <v>5</v>
       </c>
       <c r="D189" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E189" s="1">
         <v>9.7173999999999996</v>
@@ -3651,7 +3645,7 @@
         <v>5</v>
       </c>
       <c r="D190" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E190" s="1">
         <v>9.7058</v>
@@ -3668,7 +3662,7 @@
         <v>5</v>
       </c>
       <c r="D191" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E191" s="1">
         <v>9.6948000000000008</v>
@@ -3685,7 +3679,7 @@
         <v>5</v>
       </c>
       <c r="D192" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E192" s="1">
         <v>9.6841000000000008</v>
@@ -3702,7 +3696,7 @@
         <v>5</v>
       </c>
       <c r="D193" s="2">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="E193" s="1">
         <v>9.6738999999999997</v>
@@ -3719,7 +3713,7 @@
         <v>5</v>
       </c>
       <c r="D194" s="2">
-        <v>9.5000000000000001E-2</v>
+        <v>9.5</v>
       </c>
       <c r="E194" s="1">
         <v>9.6639999999999997</v>
@@ -3736,7 +3730,7 @@
         <v>4</v>
       </c>
       <c r="D195" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E195" s="1">
         <v>9.7432999999999996</v>
@@ -3753,7 +3747,7 @@
         <v>4</v>
       </c>
       <c r="D196" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E196" s="1">
         <v>9.7268000000000008</v>
@@ -3770,7 +3764,7 @@
         <v>4</v>
       </c>
       <c r="D197" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E197" s="1">
         <v>9.7112999999999996</v>
@@ -3787,7 +3781,7 @@
         <v>4</v>
       </c>
       <c r="D198" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E198" s="1">
         <v>9.6965000000000003</v>
@@ -3804,7 +3798,7 @@
         <v>4</v>
       </c>
       <c r="D199" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E199" s="1">
         <v>9.6823999999999995</v>
@@ -3821,7 +3815,7 @@
         <v>4</v>
       </c>
       <c r="D200" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E200" s="1">
         <v>9.6689000000000007</v>
@@ -3838,7 +3832,7 @@
         <v>4</v>
       </c>
       <c r="D201" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E201" s="1">
         <v>9.6559000000000008</v>
@@ -3855,7 +3849,7 @@
         <v>4</v>
       </c>
       <c r="D202" s="2">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="E202" s="1">
         <v>9.6433999999999997</v>
@@ -3872,7 +3866,7 @@
         <v>3</v>
       </c>
       <c r="D203" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E203" s="1">
         <v>9.6679999999999993</v>
@@ -3889,7 +3883,7 @@
         <v>7</v>
       </c>
       <c r="D204" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E204" s="1">
         <v>0.10252940030553762</v>
@@ -3906,7 +3900,7 @@
         <v>7</v>
       </c>
       <c r="D205" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E205" s="1">
         <v>0.10259040779687098</v>
@@ -3923,7 +3917,7 @@
         <v>7</v>
       </c>
       <c r="D206" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E206" s="1">
         <v>0.10264938051098862</v>
@@ -3940,7 +3934,7 @@
         <v>7</v>
       </c>
       <c r="D207" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E207" s="1">
         <v>0.10270420162888863</v>
@@ -3957,7 +3951,7 @@
         <v>7</v>
       </c>
       <c r="D208" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E208" s="1">
         <v>0.10275696949145575</v>
@@ -3974,7 +3968,7 @@
         <v>7</v>
       </c>
       <c r="D209" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E209" s="1">
         <v>0.10280873463009417</v>
@@ -3991,7 +3985,7 @@
         <v>7</v>
       </c>
       <c r="D210" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E210" s="1">
         <v>0.10285737795972104</v>
@@ -4008,7 +4002,7 @@
         <v>7</v>
       </c>
       <c r="D211" s="2">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="E211" s="1">
         <v>0.10290500838675817</v>
@@ -4025,7 +4019,7 @@
         <v>7</v>
       </c>
       <c r="D212" s="2">
-        <v>9.5000000000000001E-2</v>
+        <v>9.5</v>
       </c>
       <c r="E212" s="1">
         <v>0.10295056313958037</v>
@@ -4042,7 +4036,7 @@
         <v>6</v>
       </c>
       <c r="D213" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E213" s="1">
         <v>0.10247686584753492</v>
@@ -4059,7 +4053,7 @@
         <v>6</v>
       </c>
       <c r="D214" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E214" s="1">
         <v>0.10258304097166655</v>
@@ -4076,7 +4070,7 @@
         <v>6</v>
       </c>
       <c r="D215" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E215" s="1">
         <v>0.1026831096552928</v>
@@ -4093,7 +4087,7 @@
         <v>6</v>
       </c>
       <c r="D216" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E216" s="1">
         <v>0.10277703549918807</v>
@@ -4110,7 +4104,7 @@
         <v>6</v>
       </c>
       <c r="D217" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E217" s="1">
         <v>0.10286795868822779</v>
@@ -4127,7 +4121,7 @@
         <v>6</v>
       </c>
       <c r="D218" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E218" s="1">
         <v>0.10295480284155256</v>
@@ -4144,7 +4138,7 @@
         <v>6</v>
       </c>
       <c r="D219" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E219" s="1">
         <v>0.10303754688208383</v>
@@ -4161,7 +4155,7 @@
         <v>6</v>
       </c>
       <c r="D220" s="2">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="E220" s="1">
         <v>0.10311829731067482</v>
@@ -4178,7 +4172,7 @@
         <v>6</v>
       </c>
       <c r="D221" s="2">
-        <v>9.5000000000000001E-2</v>
+        <v>9.5</v>
       </c>
       <c r="E221" s="1">
         <v>0.10319597948463927</v>
@@ -4195,7 +4189,7 @@
         <v>5</v>
       </c>
       <c r="D222" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E222" s="1">
         <v>0.10249997437500641</v>
@@ -4212,7 +4206,7 @@
         <v>5</v>
       </c>
       <c r="D223" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E223" s="1">
         <v>0.10264411233371654</v>
@@ -4229,7 +4223,7 @@
         <v>5</v>
       </c>
       <c r="D224" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E224" s="1">
         <v>0.10277914816642</v>
@@ -4246,7 +4240,7 @@
         <v>5</v>
       </c>
       <c r="D225" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E225" s="1">
         <v>0.10290818531706013</v>
@@ -4263,7 +4257,7 @@
         <v>5</v>
       </c>
       <c r="D226" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E226" s="1">
         <v>0.10303117723423108</v>
@@ -4280,7 +4274,7 @@
         <v>5</v>
       </c>
       <c r="D227" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E227" s="1">
         <v>0.10314807938276188</v>
@@ -4297,7 +4291,7 @@
         <v>5</v>
       </c>
       <c r="D228" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E228" s="1">
         <v>0.10326204809946199</v>
@@ -4314,7 +4308,7 @@
         <v>5</v>
       </c>
       <c r="D229" s="2">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="E229" s="1">
         <v>0.10337092589338323</v>
@@ -4331,7 +4325,7 @@
         <v>5</v>
       </c>
       <c r="D230" s="2">
-        <v>9.5000000000000001E-2</v>
+        <v>9.5</v>
       </c>
       <c r="E230" s="1">
         <v>0.10347682119205298</v>
@@ -4348,7 +4342,7 @@
         <v>4</v>
       </c>
       <c r="D231" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E231" s="1">
         <v>0.10263463097718432</v>
@@ -4365,7 +4359,7 @@
         <v>4</v>
       </c>
       <c r="D232" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E232" s="1">
         <v>0.10280873463009417</v>
@@ -4382,7 +4376,7 @@
         <v>4</v>
       </c>
       <c r="D233" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E233" s="1">
         <v>0.10297282547135811</v>
@@ -4399,7 +4393,7 @@
         <v>4</v>
       </c>
       <c r="D234" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E234" s="1">
         <v>0.10312999535915021</v>
@@ -4416,7 +4410,7 @@
         <v>4</v>
       </c>
       <c r="D235" s="2">
-        <v>7.4999999999999997E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E235" s="1">
         <v>0.1032801784681484</v>
@@ -4433,7 +4427,7 @@
         <v>4</v>
       </c>
       <c r="D236" s="2">
-        <v>0.08</v>
+        <v>8</v>
       </c>
       <c r="E236" s="1">
         <v>0.10342438126363908</v>
@@ -4450,7 +4444,7 @@
         <v>4</v>
       </c>
       <c r="D237" s="2">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5</v>
       </c>
       <c r="E237" s="1">
         <v>0.10356362431259644</v>
@@ -4467,7 +4461,7 @@
         <v>4</v>
       </c>
       <c r="D238" s="2">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="E238" s="1">
         <v>0.10369786589791982</v>
@@ -4484,7 +4478,7 @@
         <v>3</v>
       </c>
       <c r="D239" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E239" s="1">
         <v>0.1034340091021928</v>
@@ -4501,7 +4495,7 @@
         <v>7</v>
       </c>
       <c r="D240" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E240" s="1">
         <v>5.9099000000000004</v>
@@ -4518,7 +4512,7 @@
         <v>7</v>
       </c>
       <c r="D241" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E241" s="1">
         <v>5.9146000000000001</v>
@@ -4535,7 +4529,7 @@
         <v>7</v>
       </c>
       <c r="D242" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E242" s="1">
         <v>5.9188999999999998</v>
@@ -4552,7 +4546,7 @@
         <v>7</v>
       </c>
       <c r="D243" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E243" s="1">
         <v>5.9229000000000003</v>
@@ -4569,7 +4563,7 @@
         <v>7</v>
       </c>
       <c r="D244" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E244" s="1">
         <v>5.9265999999999996</v>
@@ -4586,7 +4580,7 @@
         <v>7</v>
       </c>
       <c r="D245" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E245" s="1">
         <v>5.9302000000000001</v>
@@ -4603,7 +4597,7 @@
         <v>7</v>
       </c>
       <c r="D246" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E246" s="1">
         <v>5.9335000000000004</v>
@@ -4620,7 +4614,7 @@
         <v>7</v>
       </c>
       <c r="D247" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E247" s="1">
         <v>5.9367000000000001</v>
@@ -4637,7 +4631,7 @@
         <v>7</v>
       </c>
       <c r="D248" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E248" s="1">
         <v>5.9397000000000002</v>
@@ -4654,7 +4648,7 @@
         <v>6</v>
       </c>
       <c r="D249" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E249" s="1">
         <v>5.9081000000000001</v>
@@ -4671,7 +4665,7 @@
         <v>6</v>
       </c>
       <c r="D250" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E250" s="1">
         <v>5.9158999999999997</v>
@@ -4688,7 +4682,7 @@
         <v>6</v>
       </c>
       <c r="D251" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E251" s="1">
         <v>5.9230999999999998</v>
@@ -4705,7 +4699,7 @@
         <v>6</v>
       </c>
       <c r="D252" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E252" s="1">
         <v>5.9295999999999998</v>
@@ -4722,7 +4716,7 @@
         <v>6</v>
       </c>
       <c r="D253" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E253" s="1">
         <v>5.9356999999999998</v>
@@ -4739,7 +4733,7 @@
         <v>6</v>
       </c>
       <c r="D254" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E254" s="1">
         <v>5.9413999999999998</v>
@@ -4756,7 +4750,7 @@
         <v>6</v>
       </c>
       <c r="D255" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E255" s="1">
         <v>5.9466999999999999</v>
@@ -4773,7 +4767,7 @@
         <v>6</v>
       </c>
       <c r="D256" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E256" s="1">
         <v>5.9518000000000004</v>
@@ -4790,7 +4784,7 @@
         <v>6</v>
       </c>
       <c r="D257" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E257" s="1">
         <v>5.9565999999999999</v>
@@ -4807,7 +4801,7 @@
         <v>5</v>
       </c>
       <c r="D258" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E258" s="1">
         <v>5.8936999999999999</v>
@@ -4824,7 +4818,7 @@
         <v>5</v>
       </c>
       <c r="D259" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E259" s="1">
         <v>5.9055999999999997</v>
@@ -4841,7 +4835,7 @@
         <v>5</v>
       </c>
       <c r="D260" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E260" s="1">
         <v>5.9161999999999999</v>
@@ -4858,7 +4852,7 @@
         <v>5</v>
       </c>
       <c r="D261" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E261" s="1">
         <v>5.9259000000000004</v>
@@ -4875,7 +4869,7 @@
         <v>5</v>
       </c>
       <c r="D262" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E262" s="1">
         <v>5.9348000000000001</v>
@@ -4892,7 +4886,7 @@
         <v>5</v>
       </c>
       <c r="D263" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E263" s="1">
         <v>5.9429999999999996</v>
@@ -4909,7 +4903,7 @@
         <v>5</v>
       </c>
       <c r="D264" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E264" s="1">
         <v>5.9507000000000003</v>
@@ -4926,7 +4920,7 @@
         <v>5</v>
       </c>
       <c r="D265" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E265" s="1">
         <v>5.9580000000000002</v>
@@ -4943,7 +4937,7 @@
         <v>5</v>
       </c>
       <c r="D266" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E266" s="1">
         <v>5.9648000000000003</v>
@@ -4960,7 +4954,7 @@
         <v>4</v>
       </c>
       <c r="D267" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E267" s="1">
         <v>5.8849999999999998</v>
@@ -4977,7 +4971,7 @@
         <v>4</v>
       </c>
       <c r="D268" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E268" s="1">
         <v>5.9005000000000001</v>
@@ -4994,7 +4988,7 @@
         <v>4</v>
       </c>
       <c r="D269" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E269" s="1">
         <v>5.9142999999999999</v>
@@ -5011,7 +5005,7 @@
         <v>4</v>
       </c>
       <c r="D270" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E270" s="1">
         <v>5.9268000000000001</v>
@@ -5028,7 +5022,7 @@
         <v>4</v>
       </c>
       <c r="D271" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E271" s="1">
         <v>5.9382000000000001</v>
@@ -5045,7 +5039,7 @@
         <v>4</v>
       </c>
       <c r="D272" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E272" s="1">
         <v>5.9486999999999997</v>
@@ -5062,7 +5056,7 @@
         <v>4</v>
       </c>
       <c r="D273" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E273" s="1">
         <v>5.9584000000000001</v>
@@ -5079,7 +5073,7 @@
         <v>4</v>
       </c>
       <c r="D274" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E274" s="1">
         <v>5.9676</v>
@@ -5096,7 +5090,7 @@
         <v>4</v>
       </c>
       <c r="D275" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E275" s="1">
         <v>5.9762000000000004</v>
@@ -5113,7 +5107,7 @@
         <v>3</v>
       </c>
       <c r="D276" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E276" s="1">
         <v>5.8985000000000003</v>
@@ -5130,7 +5124,7 @@
         <v>3</v>
       </c>
       <c r="D277" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E277" s="1">
         <v>5.9249999999999998</v>
@@ -5147,7 +5141,7 @@
         <v>3</v>
       </c>
       <c r="D278" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E278" s="1">
         <v>5.9484000000000004</v>
@@ -5164,7 +5158,7 @@
         <v>3</v>
       </c>
       <c r="D279" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E279" s="1">
         <v>5.9692999999999996</v>
@@ -5181,7 +5175,7 @@
         <v>0</v>
       </c>
       <c r="D280" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E280" s="1">
         <v>5.9097999999999997</v>
@@ -5198,7 +5192,7 @@
         <v>0</v>
       </c>
       <c r="D281" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E281" s="1">
         <v>5.9451000000000001</v>
@@ -5215,7 +5209,7 @@
         <v>0</v>
       </c>
       <c r="D282" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E282" s="1">
         <v>5.976</v>
@@ -5232,7 +5226,7 @@
         <v>7</v>
       </c>
       <c r="D283" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E283" s="1">
         <v>0.16920760080542818</v>
@@ -5249,7 +5243,7 @@
         <v>7</v>
       </c>
       <c r="D284" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E284" s="1">
         <v>0.16907314104081425</v>
@@ -5266,7 +5260,7 @@
         <v>7</v>
       </c>
       <c r="D285" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E285" s="1">
         <v>0.16895031171332511</v>
@@ -5283,7 +5277,7 @@
         <v>7</v>
       </c>
       <c r="D286" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E286" s="1">
         <v>0.16883621199074778</v>
@@ -5300,7 +5294,7 @@
         <v>7</v>
       </c>
       <c r="D287" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E287" s="1">
         <v>0.16873080687071845</v>
@@ -5317,7 +5311,7 @@
         <v>7</v>
       </c>
       <c r="D288" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E288" s="1">
         <v>0.16862837678324508</v>
@@ -5334,7 +5328,7 @@
         <v>7</v>
       </c>
       <c r="D289" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E289" s="1">
         <v>0.16853459172495153</v>
@@ -5351,7 +5345,7 @@
         <v>7</v>
       </c>
       <c r="D290" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E290" s="1">
         <v>0.16844374821028518</v>
@@ -5368,7 +5362,7 @@
         <v>7</v>
       </c>
       <c r="D291" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E291" s="1">
         <v>0.16835867131336599</v>
@@ -5385,7 +5379,7 @@
         <v>6</v>
       </c>
       <c r="D292" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E292" s="1">
         <v>0.16925915268868164</v>
@@ -5402,7 +5396,7 @@
         <v>6</v>
       </c>
       <c r="D293" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E293" s="1">
         <v>0.16903598776179449</v>
@@ -5419,7 +5413,7 @@
         <v>6</v>
       </c>
       <c r="D294" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E294" s="1">
         <v>0.16883051104995694</v>
@@ -5436,7 +5430,7 @@
         <v>6</v>
       </c>
       <c r="D295" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E295" s="1">
         <v>0.16864543982730706</v>
@@ -5453,7 +5447,7 @@
         <v>6</v>
       </c>
       <c r="D296" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E296" s="1">
         <v>0.16847212628670588</v>
@@ -5470,7 +5464,7 @@
         <v>6</v>
       </c>
       <c r="D297" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E297" s="1">
         <v>0.16831049920894067</v>
@@ -5487,7 +5481,7 @@
         <v>6</v>
       </c>
       <c r="D298" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E298" s="1">
         <v>0.16816049237392167</v>
@@ -5504,7 +5498,7 @@
         <v>6</v>
       </c>
       <c r="D299" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E299" s="1">
         <v>0.16801639840048388</v>
@@ -5521,7 +5515,7 @@
         <v>6</v>
       </c>
       <c r="D300" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E300" s="1">
         <v>0.1678810059429876</v>
@@ -5538,7 +5532,7 @@
         <v>5</v>
       </c>
       <c r="D301" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E301" s="1">
         <v>0.16967270135907833</v>
@@ -5555,7 +5549,7 @@
         <v>5</v>
       </c>
       <c r="D302" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E302" s="1">
         <v>0.16933080465998376</v>
@@ -5572,7 +5566,7 @@
         <v>5</v>
       </c>
       <c r="D303" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E303" s="1">
         <v>0.16902741624691525</v>
@@ -5589,7 +5583,7 @@
         <v>5</v>
       </c>
       <c r="D304" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E304" s="1">
         <v>0.16875073828447998</v>
@@ -5606,7 +5600,7 @@
         <v>5</v>
       </c>
       <c r="D305" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E305" s="1">
         <v>0.16849767473208868</v>
@@ -5623,7 +5617,7 @@
         <v>5</v>
       </c>
       <c r="D306" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E306" s="1">
         <v>0.16826518593303047</v>
@@ -5640,7 +5634,7 @@
         <v>5</v>
       </c>
       <c r="D307" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E307" s="1">
         <v>0.16804745660174433</v>
@@ -5657,7 +5651,7 @@
         <v>5</v>
       </c>
       <c r="D308" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E308" s="1">
         <v>0.16784155756965424</v>
@@ -5674,7 +5668,7 @@
         <v>5</v>
       </c>
       <c r="D309" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E309" s="1">
         <v>0.16765021459227467</v>
@@ -5691,7 +5685,7 @@
         <v>4</v>
       </c>
       <c r="D310" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E310" s="1">
         <v>0.16992353440951571</v>
@@ -5708,7 +5702,7 @@
         <v>4</v>
       </c>
       <c r="D311" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E311" s="1">
         <v>0.16947716295229218</v>
@@ -5725,7 +5719,7 @@
         <v>4</v>
       </c>
       <c r="D312" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E312" s="1">
         <v>0.16908171719391982</v>
@@ -5742,7 +5736,7 @@
         <v>4</v>
       </c>
       <c r="D313" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E313" s="1">
         <v>0.16872511304582574</v>
@@ -5759,7 +5753,7 @@
         <v>4</v>
       </c>
       <c r="D314" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E314" s="1">
         <v>0.168401199016537</v>
@@ -5776,7 +5770,7 @@
         <v>4</v>
       </c>
       <c r="D315" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E315" s="1">
         <v>0.1681039554860726</v>
@@ -5793,7 +5787,7 @@
         <v>4</v>
       </c>
       <c r="D316" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E316" s="1">
         <v>0.16783029001074112</v>
@@ -5810,7 +5804,7 @@
         <v>4</v>
       </c>
       <c r="D317" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E317" s="1">
         <v>0.16757155305315369</v>
@@ -5827,7 +5821,7 @@
         <v>4</v>
       </c>
       <c r="D318" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E318" s="1">
         <v>0.16733041062882767</v>
@@ -5844,7 +5838,7 @@
         <v>3</v>
       </c>
       <c r="D319" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E319" s="1">
         <v>0.16953462744765618</v>
@@ -5861,7 +5855,7 @@
         <v>3</v>
       </c>
       <c r="D320" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E320" s="1">
         <v>0.16877637130801687</v>
@@ -5878,7 +5872,7 @@
         <v>3</v>
       </c>
       <c r="D321" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E321" s="1">
         <v>0.16811243359558872</v>
@@ -5895,7 +5889,7 @@
         <v>3</v>
       </c>
       <c r="D322" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E322" s="1">
         <v>0.16752383026485518</v>
@@ -5912,7 +5906,7 @@
         <v>0</v>
       </c>
       <c r="D323" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E323" s="1">
         <v>0.16921046397509223</v>
@@ -5929,7 +5923,7 @@
         <v>0</v>
       </c>
       <c r="D324" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E324" s="1">
         <v>0.16820574927251014</v>
@@ -5946,7 +5940,7 @@
         <v>0</v>
       </c>
       <c r="D325" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E325" s="1">
         <v>0.16733601070950468</v>
@@ -5963,7 +5957,7 @@
         <v>7</v>
       </c>
       <c r="D326" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E326" s="1">
         <v>8.4099000000000004</v>
@@ -5980,7 +5974,7 @@
         <v>7</v>
       </c>
       <c r="D327" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E327" s="1">
         <v>8.4038000000000004</v>
@@ -5997,7 +5991,7 @@
         <v>7</v>
       </c>
       <c r="D328" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E328" s="1">
         <v>8.3981999999999992</v>
@@ -6014,7 +6008,7 @@
         <v>7</v>
       </c>
       <c r="D329" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E329" s="1">
         <v>8.3931000000000004</v>
@@ -6031,7 +6025,7 @@
         <v>7</v>
       </c>
       <c r="D330" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E330" s="1">
         <v>8.3881999999999994</v>
@@ -6048,7 +6042,7 @@
         <v>7</v>
       </c>
       <c r="D331" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E331" s="1">
         <v>8.3836999999999993</v>
@@ -6065,7 +6059,7 @@
         <v>7</v>
       </c>
       <c r="D332" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E332" s="1">
         <v>8.3795000000000002</v>
@@ -6082,7 +6076,7 @@
         <v>7</v>
       </c>
       <c r="D333" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E333" s="1">
         <v>8.3755000000000006</v>
@@ -6099,7 +6093,7 @@
         <v>7</v>
       </c>
       <c r="D334" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E334" s="1">
         <v>8.3716000000000008</v>
@@ -6116,7 +6110,7 @@
         <v>6</v>
       </c>
       <c r="D335" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E335" s="1">
         <v>8.4215999999999998</v>
@@ -6133,7 +6127,7 @@
         <v>6</v>
       </c>
       <c r="D336" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E336" s="1">
         <v>8.4110999999999994</v>
@@ -6150,7 +6144,7 @@
         <v>6</v>
       </c>
       <c r="D337" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E337" s="1">
         <v>8.4015000000000004</v>
@@ -6167,7 +6161,7 @@
         <v>6</v>
       </c>
       <c r="D338" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E338" s="1">
         <v>8.3926999999999996</v>
@@ -6184,7 +6178,7 @@
         <v>6</v>
       </c>
       <c r="D339" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E339" s="1">
         <v>8.3846000000000007</v>
@@ -6201,7 +6195,7 @@
         <v>6</v>
       </c>
       <c r="D340" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E340" s="1">
         <v>8.3771000000000004</v>
@@ -6218,7 +6212,7 @@
         <v>6</v>
       </c>
       <c r="D341" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E341" s="1">
         <v>8.3698999999999995</v>
@@ -6235,7 +6229,7 @@
         <v>6</v>
       </c>
       <c r="D342" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E342" s="1">
         <v>8.3632000000000009</v>
@@ -6252,7 +6246,7 @@
         <v>6</v>
       </c>
       <c r="D343" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E343" s="1">
         <v>8.3567999999999998</v>
@@ -6269,7 +6263,7 @@
         <v>5</v>
       </c>
       <c r="D344" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E344" s="1">
         <v>8.4285999999999994</v>
@@ -6286,7 +6280,7 @@
         <v>5</v>
       </c>
       <c r="D345" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E345" s="1">
         <v>8.4139999999999997</v>
@@ -6303,7 +6297,7 @@
         <v>5</v>
       </c>
       <c r="D346" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E346" s="1">
         <v>8.4009</v>
@@ -6320,7 +6314,7 @@
         <v>5</v>
       </c>
       <c r="D347" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E347" s="1">
         <v>8.3888999999999996</v>
@@ -6337,7 +6331,7 @@
         <v>5</v>
       </c>
       <c r="D348" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E348" s="1">
         <v>8.3779000000000003</v>
@@ -6354,7 +6348,7 @@
         <v>5</v>
       </c>
       <c r="D349" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E349" s="1">
         <v>8.3675999999999995</v>
@@ -6371,7 +6365,7 @@
         <v>5</v>
       </c>
       <c r="D350" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E350" s="1">
         <v>8.3580000000000005</v>
@@ -6388,7 +6382,7 @@
         <v>5</v>
       </c>
       <c r="D351" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E351" s="1">
         <v>8.3488000000000007</v>
@@ -6405,7 +6399,7 @@
         <v>5</v>
       </c>
       <c r="D352" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E352" s="1">
         <v>8.3400999999999996</v>
@@ -6422,7 +6416,7 @@
         <v>4</v>
       </c>
       <c r="D353" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E353" s="1">
         <v>8.4289000000000005</v>
@@ -6439,7 +6433,7 @@
         <v>4</v>
       </c>
       <c r="D354" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E354" s="1">
         <v>8.4109999999999996</v>
@@ -6456,7 +6450,7 @@
         <v>4</v>
       </c>
       <c r="D355" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E355" s="1">
         <v>8.3948999999999998</v>
@@ -6473,7 +6467,7 @@
         <v>4</v>
       </c>
       <c r="D356" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E356" s="1">
         <v>8.3802000000000003</v>
@@ -6490,7 +6484,7 @@
         <v>4</v>
       </c>
       <c r="D357" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E357" s="1">
         <v>8.3666999999999998</v>
@@ -6507,7 +6501,7 @@
         <v>4</v>
       </c>
       <c r="D358" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E358" s="1">
         <v>8.3541000000000007</v>
@@ -6524,7 +6518,7 @@
         <v>4</v>
       </c>
       <c r="D359" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E359" s="1">
         <v>8.3422000000000001</v>
@@ -6541,7 +6535,7 @@
         <v>4</v>
       </c>
       <c r="D360" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E360" s="1">
         <v>8.3309999999999995</v>
@@ -6558,7 +6552,7 @@
         <v>4</v>
       </c>
       <c r="D361" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E361" s="1">
         <v>8.3201999999999998</v>
@@ -6575,7 +6569,7 @@
         <v>3</v>
       </c>
       <c r="D362" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E362" s="1">
         <v>8.4350000000000005</v>
@@ -6592,7 +6586,7 @@
         <v>3</v>
       </c>
       <c r="D363" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E363" s="1">
         <v>8.4037000000000006</v>
@@ -6609,7 +6603,7 @@
         <v>3</v>
       </c>
       <c r="D364" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E364" s="1">
         <v>8.3755000000000006</v>
@@ -6626,7 +6620,7 @@
         <v>3</v>
       </c>
       <c r="D365" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E365" s="1">
         <v>8.3495000000000008</v>
@@ -6643,7 +6637,7 @@
         <v>3</v>
       </c>
       <c r="D366" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E366" s="1">
         <v>8.3254000000000001</v>
@@ -6660,7 +6654,7 @@
         <v>0</v>
       </c>
       <c r="D367" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E367" s="1">
         <v>8.4295000000000009</v>
@@ -6677,7 +6671,7 @@
         <v>0</v>
       </c>
       <c r="D368" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E368" s="1">
         <v>8.3880999999999997</v>
@@ -6694,7 +6688,7 @@
         <v>0</v>
       </c>
       <c r="D369" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E369" s="1">
         <v>8.3505000000000003</v>
@@ -6711,7 +6705,7 @@
         <v>0</v>
       </c>
       <c r="D370" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E370" s="1">
         <v>8.3156999999999996</v>
@@ -6728,7 +6722,7 @@
         <v>7</v>
       </c>
       <c r="D371" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E371" s="1">
         <v>0.11890747809129716</v>
@@ -6745,7 +6739,7 @@
         <v>7</v>
       </c>
       <c r="D372" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E372" s="1">
         <v>0.11899378852423903</v>
@@ -6762,7 +6756,7 @@
         <v>7</v>
       </c>
       <c r="D373" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E373" s="1">
         <v>0.11907313471934464</v>
@@ -6779,7 +6773,7 @@
         <v>7</v>
       </c>
       <c r="D374" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E374" s="1">
         <v>0.11914548855607582</v>
@@ -6796,7 +6790,7 @@
         <v>7</v>
       </c>
       <c r="D375" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E375" s="1">
         <v>0.11921508786151976</v>
@@ -6813,7 +6807,7 @@
         <v>7</v>
       </c>
       <c r="D376" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E376" s="1">
         <v>0.11927907725705834</v>
@@ -6830,7 +6824,7 @@
         <v>7</v>
       </c>
       <c r="D377" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E377" s="1">
         <v>0.11933886270063845</v>
@@ -6847,7 +6841,7 @@
         <v>7</v>
       </c>
       <c r="D378" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E378" s="1">
         <v>0.11939585696376336</v>
@@ -6864,7 +6858,7 @@
         <v>7</v>
       </c>
       <c r="D379" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E379" s="1">
         <v>0.11945147880930765</v>
@@ -6881,7 +6875,7 @@
         <v>6</v>
       </c>
       <c r="D380" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E380" s="1">
         <v>0.11874228175168615</v>
@@ -6898,7 +6892,7 @@
         <v>6</v>
       </c>
       <c r="D381" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E381" s="1">
         <v>0.11889051372590982</v>
@@ -6915,7 +6909,7 @@
         <v>6</v>
       </c>
       <c r="D382" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E382" s="1">
         <v>0.11902636433970123</v>
@@ -6932,7 +6926,7 @@
         <v>6</v>
       </c>
       <c r="D383" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E383" s="1">
         <v>0.1191511670856816</v>
@@ -6949,7 +6943,7 @@
         <v>6</v>
       </c>
       <c r="D384" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E384" s="1">
         <v>0.11926627388307133</v>
@@ -6966,7 +6960,7 @@
         <v>6</v>
       </c>
       <c r="D385" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E385" s="1">
         <v>0.11937305272707738</v>
@@ -6983,7 +6977,7 @@
         <v>6</v>
       </c>
       <c r="D386" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E386" s="1">
         <v>0.11947574045090145</v>
@@ -7000,7 +6994,7 @@
         <v>6</v>
       </c>
       <c r="D387" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E387" s="1">
         <v>0.11957145590204706</v>
@@ -7017,7 +7011,7 @@
         <v>6</v>
       </c>
       <c r="D388" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E388" s="1">
         <v>0.11966302891058779</v>
@@ -7034,7 +7028,7 @@
         <v>5</v>
       </c>
       <c r="D389" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E389" s="1">
         <v>0.11864366561469283</v>
@@ -7051,7 +7045,7 @@
         <v>5</v>
       </c>
       <c r="D390" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E390" s="1">
         <v>0.11884953648680771</v>
@@ -7068,7 +7062,7 @@
         <v>5</v>
       </c>
       <c r="D391" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E391" s="1">
         <v>0.1190348653120499</v>
@@ -7085,7 +7079,7 @@
         <v>5</v>
       </c>
       <c r="D392" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E392" s="1">
         <v>0.11920514012564222</v>
@@ -7102,7 +7096,7 @@
         <v>5</v>
       </c>
       <c r="D393" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E393" s="1">
         <v>0.11936165387507609</v>
@@ -7119,7 +7113,7 @@
         <v>5</v>
       </c>
       <c r="D394" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E394" s="1">
         <v>0.11950858071609542</v>
@@ -7136,7 +7130,7 @@
         <v>5</v>
       </c>
       <c r="D395" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E395" s="1">
         <v>0.11964584828906435</v>
@@ -7153,7 +7147,7 @@
         <v>5</v>
       </c>
       <c r="D396" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E396" s="1">
         <v>0.1197776926025297</v>
@@ -7170,7 +7164,7 @@
         <v>5</v>
       </c>
       <c r="D397" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E397" s="1">
         <v>0.11990263905708565</v>
@@ -7187,7 +7181,7 @@
         <v>4</v>
       </c>
       <c r="D398" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E398" s="1">
         <v>0.11863944286917628</v>
@@ -7204,7 +7198,7 @@
         <v>4</v>
       </c>
       <c r="D399" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E399" s="1">
         <v>0.11889192723814053</v>
@@ -7221,7 +7215,7 @@
         <v>4</v>
       </c>
       <c r="D400" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E400" s="1">
         <v>0.11911994186946837</v>
@@ -7238,7 +7232,7 @@
         <v>4</v>
       </c>
       <c r="D401" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E401" s="1">
         <v>0.11932889429846542</v>
@@ -7255,7 +7249,7 @@
         <v>4</v>
       </c>
       <c r="D402" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E402" s="1">
         <v>0.11952143616957701</v>
@@ -7272,7 +7266,7 @@
         <v>4</v>
       </c>
       <c r="D403" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E403" s="1">
         <v>0.11970170335523873</v>
@@ -7289,7 +7283,7 @@
         <v>4</v>
       </c>
       <c r="D404" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E404" s="1">
         <v>0.11987245570712761</v>
@@ -7306,7 +7300,7 @@
         <v>4</v>
       </c>
       <c r="D405" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.5</v>
       </c>
       <c r="E405" s="1">
         <v>0.12003360941063498</v>
@@ -7323,7 +7317,7 @@
         <v>4</v>
       </c>
       <c r="D406" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="E406" s="1">
         <v>0.12018941852359319</v>
@@ -7340,7 +7334,7 @@
         <v>3</v>
       </c>
       <c r="D407" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E407" s="1">
         <v>0.11855364552459988</v>
@@ -7357,7 +7351,7 @@
         <v>3</v>
       </c>
       <c r="D408" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E408" s="1">
         <v>0.11899520449325891</v>
@@ -7374,7 +7368,7 @@
         <v>3</v>
       </c>
       <c r="D409" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E409" s="1">
         <v>0.11939585696376336</v>
@@ -7391,7 +7385,7 @@
         <v>3</v>
       </c>
       <c r="D410" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E410" s="1">
         <v>0.11976765075753038</v>
@@ -7408,7 +7402,7 @@
         <v>3</v>
       </c>
       <c r="D411" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E411" s="1">
         <v>0.12011434886011482</v>
@@ -7425,7 +7419,7 @@
         <v>0</v>
       </c>
       <c r="D412" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E412" s="1">
         <v>0.11863099827985052</v>
@@ -7442,7 +7436,7 @@
         <v>0</v>
       </c>
       <c r="D413" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E413" s="1">
         <v>0.11921650910218047</v>
@@ -7459,7 +7453,7 @@
         <v>0</v>
       </c>
       <c r="D414" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E414" s="1">
         <v>0.11975330818513862</v>
@@ -7476,7 +7470,7 @@
         <v>0</v>
       </c>
       <c r="D415" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E415" s="1">
         <v>0.12025445843404645</v>
@@ -7493,7 +7487,7 @@
         <v>7</v>
       </c>
       <c r="D416" s="2">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="E416" s="1">
         <v>1.1326000000000001</v>
@@ -7510,7 +7504,7 @@
         <v>7</v>
       </c>
       <c r="D417" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5</v>
       </c>
       <c r="E417" s="1">
         <v>1.1335999999999999</v>
@@ -7527,7 +7521,7 @@
         <v>7</v>
       </c>
       <c r="D418" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E418" s="1">
         <v>1.1344000000000001</v>
@@ -7544,7 +7538,7 @@
         <v>7</v>
       </c>
       <c r="D419" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E419" s="1">
         <v>1.1352</v>
@@ -7561,7 +7555,7 @@
         <v>7</v>
       </c>
       <c r="D420" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E420" s="1">
         <v>1.1357999999999999</v>
@@ -7578,7 +7572,7 @@
         <v>7</v>
       </c>
       <c r="D421" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E421" s="1">
         <v>1.1365000000000001</v>
@@ -7595,7 +7589,7 @@
         <v>7</v>
       </c>
       <c r="D422" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E422" s="1">
         <v>1.137</v>
@@ -7612,7 +7606,7 @@
         <v>7</v>
       </c>
       <c r="D423" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E423" s="1">
         <v>1.1375</v>
@@ -7629,7 +7623,7 @@
         <v>7</v>
       </c>
       <c r="D424" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E424" s="1">
         <v>1.1379999999999999</v>
@@ -7646,7 +7640,7 @@
         <v>6</v>
       </c>
       <c r="D425" s="2">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="E425" s="1">
         <v>1.1301000000000001</v>
@@ -7663,7 +7657,7 @@
         <v>6</v>
       </c>
       <c r="D426" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5</v>
       </c>
       <c r="E426" s="1">
         <v>1.1318999999999999</v>
@@ -7680,7 +7674,7 @@
         <v>6</v>
       </c>
       <c r="D427" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E427" s="1">
         <v>1.1333</v>
@@ -7697,7 +7691,7 @@
         <v>6</v>
       </c>
       <c r="D428" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E428" s="1">
         <v>1.1345000000000001</v>
@@ -7714,7 +7708,7 @@
         <v>6</v>
       </c>
       <c r="D429" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E429" s="1">
         <v>1.1355999999999999</v>
@@ -7731,7 +7725,7 @@
         <v>6</v>
       </c>
       <c r="D430" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E430" s="1">
         <v>1.1366000000000001</v>
@@ -7748,7 +7742,7 @@
         <v>6</v>
       </c>
       <c r="D431" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E431" s="1">
         <v>1.1375999999999999</v>
@@ -7765,7 +7759,7 @@
         <v>6</v>
       </c>
       <c r="D432" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E432" s="1">
         <v>1.1384000000000001</v>
@@ -7782,7 +7776,7 @@
         <v>6</v>
       </c>
       <c r="D433" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E433" s="1">
         <v>1.1393</v>
@@ -7799,7 +7793,7 @@
         <v>5</v>
       </c>
       <c r="D434" s="2">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="E434" s="1">
         <v>1.1279999999999999</v>
@@ -7816,7 +7810,7 @@
         <v>5</v>
       </c>
       <c r="D435" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5</v>
       </c>
       <c r="E435" s="1">
         <v>1.1304000000000001</v>
@@ -7833,7 +7827,7 @@
         <v>5</v>
       </c>
       <c r="D436" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E436" s="1">
         <v>1.1324000000000001</v>
@@ -7850,7 +7844,7 @@
         <v>5</v>
       </c>
       <c r="D437" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E437" s="1">
         <v>1.1341000000000001</v>
@@ -7867,7 +7861,7 @@
         <v>5</v>
       </c>
       <c r="D438" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E438" s="1">
         <v>1.1355999999999999</v>
@@ -7884,7 +7878,7 @@
         <v>5</v>
       </c>
       <c r="D439" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E439" s="1">
         <v>1.137</v>
@@ -7901,7 +7895,7 @@
         <v>5</v>
       </c>
       <c r="D440" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E440" s="1">
         <v>1.1383000000000001</v>
@@ -7918,7 +7912,7 @@
         <v>5</v>
       </c>
       <c r="D441" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E441" s="1">
         <v>1.1395</v>
@@ -7935,7 +7929,7 @@
         <v>5</v>
       </c>
       <c r="D442" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E442" s="1">
         <v>1.1406000000000001</v>
@@ -7952,7 +7946,7 @@
         <v>4</v>
       </c>
       <c r="D443" s="2">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="E443" s="1">
         <v>1.1254</v>
@@ -7969,7 +7963,7 @@
         <v>4</v>
       </c>
       <c r="D444" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5</v>
       </c>
       <c r="E444" s="1">
         <v>1.1287</v>
@@ -7986,7 +7980,7 @@
         <v>4</v>
       </c>
       <c r="D445" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E445" s="1">
         <v>1.1313</v>
@@ -8003,7 +7997,7 @@
         <v>4</v>
       </c>
       <c r="D446" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E446" s="1">
         <v>1.1335</v>
@@ -8020,7 +8014,7 @@
         <v>4</v>
       </c>
       <c r="D447" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E447" s="1">
         <v>1.1355</v>
@@ -8037,7 +8031,7 @@
         <v>4</v>
       </c>
       <c r="D448" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E448" s="1">
         <v>1.1373</v>
@@ -8054,7 +8048,7 @@
         <v>4</v>
       </c>
       <c r="D449" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E449" s="1">
         <v>1.1389</v>
@@ -8071,7 +8065,7 @@
         <v>4</v>
       </c>
       <c r="D450" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E450" s="1">
         <v>1.1404000000000001</v>
@@ -8088,7 +8082,7 @@
         <v>4</v>
       </c>
       <c r="D451" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E451" s="1">
         <v>1.1417999999999999</v>
@@ -8105,7 +8099,7 @@
         <v>3</v>
       </c>
       <c r="D452" s="2">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="E452" s="1">
         <v>1.1188</v>
@@ -8122,7 +8116,7 @@
         <v>3</v>
       </c>
       <c r="D453" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5</v>
       </c>
       <c r="E453" s="1">
         <v>1.1248</v>
@@ -8139,7 +8133,7 @@
         <v>3</v>
       </c>
       <c r="D454" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E454" s="1">
         <v>1.1296999999999999</v>
@@ -8156,7 +8150,7 @@
         <v>3</v>
       </c>
       <c r="D455" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E455" s="1">
         <v>1.1337999999999999</v>
@@ -8173,7 +8167,7 @@
         <v>3</v>
       </c>
       <c r="D456" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E456" s="1">
         <v>1.1374</v>
@@ -8190,7 +8184,7 @@
         <v>3</v>
       </c>
       <c r="D457" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E457" s="1">
         <v>1.1406000000000001</v>
@@ -8207,7 +8201,7 @@
         <v>3</v>
       </c>
       <c r="D458" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E458" s="1">
         <v>1.1435</v>
@@ -8224,7 +8218,7 @@
         <v>0</v>
       </c>
       <c r="D459" s="2">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="E459" s="1">
         <v>1.1147</v>
@@ -8241,7 +8235,7 @@
         <v>0</v>
       </c>
       <c r="D460" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5</v>
       </c>
       <c r="E460" s="1">
         <v>1.123</v>
@@ -8258,7 +8252,7 @@
         <v>0</v>
       </c>
       <c r="D461" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E461" s="1">
         <v>1.1295999999999999</v>
@@ -8275,7 +8269,7 @@
         <v>0</v>
       </c>
       <c r="D462" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E462" s="1">
         <v>1.1351</v>
@@ -8292,7 +8286,7 @@
         <v>0</v>
       </c>
       <c r="D463" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E463" s="1">
         <v>1.1398999999999999</v>
@@ -8309,7 +8303,7 @@
         <v>0</v>
       </c>
       <c r="D464" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E464" s="1">
         <v>1.1440999999999999</v>
@@ -8326,7 +8320,7 @@
         <v>7</v>
       </c>
       <c r="D465" s="2">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="E465" s="1">
         <v>0.88292424509977041</v>
@@ -8343,7 +8337,7 @@
         <v>7</v>
       </c>
       <c r="D466" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5</v>
       </c>
       <c r="E466" s="1">
         <v>0.88214537755822164</v>
@@ -8360,7 +8354,7 @@
         <v>7</v>
       </c>
       <c r="D467" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E467" s="1">
         <v>0.88152327221438642</v>
@@ -8377,7 +8371,7 @@
         <v>7</v>
       </c>
       <c r="D468" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E468" s="1">
         <v>0.88090204369274139</v>
@@ -8394,7 +8388,7 @@
         <v>7</v>
       </c>
       <c r="D469" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E469" s="1">
         <v>0.88043669660151447</v>
@@ -8411,7 +8405,7 @@
         <v>7</v>
       </c>
       <c r="D470" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E470" s="1">
         <v>0.87989441267047952</v>
@@ -8428,7 +8422,7 @@
         <v>7</v>
       </c>
       <c r="D471" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E471" s="1">
         <v>0.87950747581354438</v>
@@ -8445,7 +8439,7 @@
         <v>7</v>
       </c>
       <c r="D472" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E472" s="1">
         <v>0.87912087912087911</v>
@@ -8462,7 +8456,7 @@
         <v>7</v>
       </c>
       <c r="D473" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E473" s="1">
         <v>0.87873462214411258</v>
@@ -8479,7 +8473,7 @@
         <v>6</v>
       </c>
       <c r="D474" s="2">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="E474" s="1">
         <v>0.88487744447394023</v>
@@ -8496,7 +8490,7 @@
         <v>6</v>
       </c>
       <c r="D475" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5</v>
       </c>
       <c r="E475" s="1">
         <v>0.88347027122537336</v>
@@ -8513,7 +8507,7 @@
         <v>6</v>
       </c>
       <c r="D476" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E476" s="1">
         <v>0.8823788934968676</v>
@@ -8530,7 +8524,7 @@
         <v>6</v>
       </c>
       <c r="D477" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E477" s="1">
         <v>0.88144557073600704</v>
@@ -8547,7 +8541,7 @@
         <v>6</v>
       </c>
       <c r="D478" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E478" s="1">
         <v>0.88059175766114839</v>
@@ -8564,7 +8558,7 @@
         <v>6</v>
       </c>
       <c r="D479" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E479" s="1">
         <v>0.87981699806440261</v>
@@ -8581,7 +8575,7 @@
         <v>6</v>
       </c>
       <c r="D480" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E480" s="1">
         <v>0.8790436005625879</v>
@@ -8598,7 +8592,7 @@
         <v>6</v>
       </c>
       <c r="D481" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E481" s="1">
         <v>0.87842586085734353</v>
@@ -8615,7 +8609,7 @@
         <v>6</v>
       </c>
       <c r="D482" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E482" s="1">
         <v>0.87773194066532079</v>
@@ -8632,7 +8626,7 @@
         <v>5</v>
       </c>
       <c r="D483" s="2">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="E483" s="1">
         <v>0.88652482269503552</v>
@@ -8649,7 +8643,7 @@
         <v>5</v>
       </c>
       <c r="D484" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5</v>
       </c>
       <c r="E484" s="1">
         <v>0.88464260438782727</v>
@@ -8666,7 +8660,7 @@
         <v>5</v>
       </c>
       <c r="D485" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E485" s="1">
         <v>0.8830801836806782</v>
@@ -8683,7 +8677,7 @@
         <v>5</v>
       </c>
       <c r="D486" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E486" s="1">
         <v>0.88175645886606113</v>
@@ -8700,7 +8694,7 @@
         <v>5</v>
       </c>
       <c r="D487" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E487" s="1">
         <v>0.88059175766114839</v>
@@ -8717,7 +8711,7 @@
         <v>5</v>
       </c>
       <c r="D488" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E488" s="1">
         <v>0.87950747581354438</v>
@@ -8734,7 +8728,7 @@
         <v>5</v>
       </c>
       <c r="D489" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E489" s="1">
         <v>0.87850303083545633</v>
@@ -8751,7 +8745,7 @@
         <v>5</v>
       </c>
       <c r="D490" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E490" s="1">
         <v>0.87757788503729706</v>
@@ -8768,7 +8762,7 @@
         <v>5</v>
       </c>
       <c r="D491" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E491" s="1">
         <v>0.87673154480098192</v>
@@ -8785,7 +8779,7 @@
         <v>4</v>
       </c>
       <c r="D492" s="2">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="E492" s="1">
         <v>0.88857295183934604</v>
@@ -8802,7 +8796,7 @@
         <v>4</v>
       </c>
       <c r="D493" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5</v>
       </c>
       <c r="E493" s="1">
         <v>0.8859750155045627</v>
@@ -8819,7 +8813,7 @@
         <v>4</v>
       </c>
       <c r="D494" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E494" s="1">
         <v>0.88393883143286489</v>
@@ -8836,7 +8830,7 @@
         <v>4</v>
       </c>
       <c r="D495" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E495" s="1">
         <v>0.88222320247022501</v>
@@ -8853,7 +8847,7 @@
         <v>4</v>
       </c>
       <c r="D496" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E496" s="1">
         <v>0.8806693086745927</v>
@@ -8870,7 +8864,7 @@
         <v>4</v>
       </c>
       <c r="D497" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E497" s="1">
         <v>0.8792754770069463</v>
@@ -8887,7 +8881,7 @@
         <v>4</v>
       </c>
       <c r="D498" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E498" s="1">
         <v>0.87804021424181222</v>
@@ -8904,7 +8898,7 @@
         <v>4</v>
       </c>
       <c r="D499" s="2">
-        <v>5.5E-2</v>
+        <v>5.5</v>
       </c>
       <c r="E499" s="1">
         <v>0.87688530340231496</v>
@@ -8921,7 +8915,7 @@
         <v>4</v>
       </c>
       <c r="D500" s="2">
-        <v>0.06</v>
+        <v>6</v>
       </c>
       <c r="E500" s="1">
         <v>0.87581012436503769</v>
@@ -8938,7 +8932,7 @@
         <v>3</v>
       </c>
       <c r="D501" s="2">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="E501" s="1">
         <v>0.89381480157311399</v>
@@ -8955,7 +8949,7 @@
         <v>3</v>
       </c>
       <c r="D502" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5</v>
       </c>
       <c r="E502" s="1">
         <v>0.88904694167852061</v>
@@ -8972,7 +8966,7 @@
         <v>3</v>
       </c>
       <c r="D503" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E503" s="1">
         <v>0.88519075860848018</v>
@@ -8989,7 +8983,7 @@
         <v>3</v>
       </c>
       <c r="D504" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E504" s="1">
         <v>0.88198976891868064</v>
@@ -9006,7 +9000,7 @@
         <v>3</v>
       </c>
       <c r="D505" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E505" s="1">
         <v>0.87919817126780375</v>
@@ -9023,7 +9017,7 @@
         <v>3</v>
       </c>
       <c r="D506" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E506" s="1">
         <v>0.87673154480098192</v>
@@ -9040,7 +9034,7 @@
         <v>3</v>
       </c>
       <c r="D507" s="2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="E507" s="1">
         <v>0.87450808919982514</v>
@@ -9057,7 +9051,7 @@
         <v>0</v>
       </c>
       <c r="D508" s="2">
-        <v>0.02</v>
+        <v>2</v>
       </c>
       <c r="E508" s="1">
         <v>0.89710235937920513</v>
@@ -9074,7 +9068,7 @@
         <v>0</v>
       </c>
       <c r="D509" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2.5</v>
       </c>
       <c r="E509" s="1">
         <v>0.89047195013357083</v>
@@ -9091,7 +9085,7 @@
         <v>0</v>
       </c>
       <c r="D510" s="2">
-        <v>0.03</v>
+        <v>3</v>
       </c>
       <c r="E510" s="1">
         <v>0.88526912181303119</v>
@@ -9108,7 +9102,7 @@
         <v>0</v>
       </c>
       <c r="D511" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="E511" s="1">
         <v>0.88097964937009954</v>
@@ -9125,7 +9119,7 @@
         <v>0</v>
       </c>
       <c r="D512" s="2">
-        <v>0.04</v>
+        <v>4</v>
       </c>
       <c r="E512" s="1">
         <v>0.8772699359592947</v>
@@ -9142,7 +9136,7 @@
         <v>0</v>
       </c>
       <c r="D513" s="2">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5</v>
       </c>
       <c r="E513" s="1">
         <v>0.87404947120007004</v>

</xml_diff>